<commit_message>
Updated on 1402-02-22 by https://github.com/imahdimir/u-d-Iran-RiskFree-Rate-Monthly
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>JMonth</t>
   </si>
   <si>
     <t>RiskFree-Rate-APR</t>
+  </si>
+  <si>
+    <t>RiskFree-Rate-Daily</t>
   </si>
   <si>
     <t>1399-04</t>
@@ -800,1146 +803,1572 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B142"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0.0004067128362559291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>0.0004996358909556964</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>18</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>18</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <v>18</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>18</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>18</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>18</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64">
+        <v>0.0004535670454468566</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>22</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>22</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>22</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>22</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>22</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B71">
         <v>22</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>22</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B74">
         <v>22</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>22</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>22</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77">
+        <v>0.0005449453020442974</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>17</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>17</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B81">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B82">
         <v>17</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>17</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>17</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>17</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>17</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>17</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B90">
         <v>17</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B91">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B97">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B98">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B99">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B100">
         <v>17</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B101">
         <v>17</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="C101">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B102">
         <v>17</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B103">
         <v>17</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="C103">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B104">
         <v>17</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B105">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="C105">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B106">
         <v>17</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="C106">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B107">
         <v>17</v>
       </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="C107">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B108">
         <v>17</v>
       </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="C108">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B109">
         <v>17</v>
       </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="C109">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B110">
         <v>17</v>
       </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="C110">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B111">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="C111">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B112">
         <v>17</v>
       </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="C112">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B113">
         <v>17</v>
       </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="C113">
+        <v>0.0004302397836104532</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B114">
         <v>14</v>
       </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="C114">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B115">
         <v>14</v>
       </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="C115">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B116">
         <v>14</v>
       </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="C116">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>14</v>
       </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="C117">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B118">
         <v>14</v>
       </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="C118">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B119">
         <v>14</v>
       </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="C119">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B120">
         <v>14</v>
       </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="C120">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B121">
         <v>14</v>
       </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="C121">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B122">
         <v>14</v>
       </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="C122">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B123">
         <v>14</v>
       </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="C123">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B124">
         <v>14</v>
       </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="C124">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B125">
         <v>14</v>
       </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="C125">
+        <v>0.0003590459824236447</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B126">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="C126">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B127">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="C127">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B128">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="C128">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B129">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="C129">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B130">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="C130">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B131">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="C131">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B132">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="C132">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B133">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="C133">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B134">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="C134">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B135">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="C135">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B136">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="C136">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B137">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="C137">
+        <v>0.0003710404267127654</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B138">
         <v>15</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="C138">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B139">
         <v>15</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="C139">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B140">
         <v>15</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="C140">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B141">
         <v>15</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="C141">
+        <v>0.0003829827503389893</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B142">
         <v>15</v>
+      </c>
+      <c r="C142">
+        <v>0.0003829827503389893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>